<commit_message>
created database, performed ELT pipeline, update progress report
</commit_message>
<xml_diff>
--- a/DocumentsAndReports/0. WorkLog_Charts.xlsx
+++ b/DocumentsAndReports/0. WorkLog_Charts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qhung\Videos\CSIS4495 - Applied Research  Project\W26_4495_S2_HughT\DocumentsAndReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E343ED-4F51-41D1-9EA3-191D752C566D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408518D8-E9CA-43B5-B9FA-37D5CA288550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="972" yWindow="696" windowWidth="21600" windowHeight="11232" xr2:uid="{E067A1E6-0DC4-42DD-AAF8-D95EFF7A112F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>January</t>
   </si>
@@ -96,20 +96,170 @@
     <t>Actions</t>
   </si>
   <si>
-    <t>submitted the proposal</t>
-  </si>
-  <si>
-    <t>created repo on GitHub</t>
-  </si>
-  <si>
-    <t>researched dataset</t>
+    <t>“customer’s review corpus in csv is considered as structured or unstructured data?”</t>
+  </si>
+  <si>
+    <t>“any legal issues of the scraping?”</t>
+  </si>
+  <si>
+    <t>“explain in details these statements”</t>
+  </si>
+  <si>
+    <t>“why used view instead of creating another analysis table? ”</t>
+  </si>
+  <si>
+    <t>“wording these paragraphs”</t>
+  </si>
+  <si>
+    <t>“what types of corpus of customer’s reviews could be?”</t>
+  </si>
+  <si>
+    <t>“review this dataset to see whether is it meet requirements of my project?”</t>
+  </si>
+  <si>
+    <t>“how to connect backend and SQL server by python?”</t>
+  </si>
+  <si>
+    <t>“any syntax issue of this table creation?”</t>
+  </si>
+  <si>
+    <t>“how to inject data from csv into SQL server by python?”</t>
+  </si>
+  <si>
+    <t>“any wrong syntax or unlogic of this function? and correct it”</t>
+  </si>
+  <si>
+    <t>“why should have dim and fact tables?”</t>
+  </si>
+  <si>
+    <t>“dim &amp; fact are for normalization purpose, is it right?”</t>
+  </si>
+  <si>
+    <t>“why don’t use data directly from the clean tables, instead of creating new analysis tables?”</t>
+  </si>
+  <si>
+    <t>-  Searched for datasets that could be used for the project. Websites such as Kaggle and Google Dataset Search were checked. The focus was on finding data with sales information and customer reviews</t>
+  </si>
+  <si>
+    <t>-  ChatGPT’s prompts:</t>
+  </si>
+  <si>
+    <t>-  Continued searching for datasets on Kaggle, the UCI Machine Learning Repository, and Harvard Dataverse. Different datasets were reviewed to see if they met the project requirements</t>
+  </si>
+  <si>
+    <t>-  Looked for more datasets on Data.gov and Kaggle</t>
+  </si>
+  <si>
+    <t>-  Researched data scraping techniques from web</t>
+  </si>
+  <si>
+    <t>-  Selected a dataset from Kaggle due to time limits</t>
+  </si>
+  <si>
+    <t>-  Set up environments (VSC, SQL Server Management System, ODBC)</t>
+  </si>
+  <si>
+    <t>-  Created IBP database in SQL Server</t>
+  </si>
+  <si>
+    <t>-  Created schemas for raw dataset</t>
+  </si>
+  <si>
+    <t>-  Researched inserting the raw data into the database by Python</t>
+  </si>
+  <si>
+    <t>-  Loaded the raw sales and review data into the database using Python. Checked the results to make sure the data was loaded correctly.</t>
+  </si>
+  <si>
+    <t>-  Studied data cleaning methods using Python.</t>
+  </si>
+  <si>
+    <t>-  Created clean tables using dimension and fact tables in SQL Server.</t>
+  </si>
+  <si>
+    <t>-  Transformed raw data into clean data</t>
+  </si>
+  <si>
+    <t>-  Studied how to prepare data for Power BI.</t>
+  </si>
+  <si>
+    <t>-  Created analysis tables and a summary view in SQL Server.</t>
+  </si>
+  <si>
+    <t>-  Drafted the project progress report</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>“suggest sources of dataset as the project requirements”</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>“how to scrap data of sales and client’s review from a web”</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>“which dependencies must be installed for my project?”</t>
+    </r>
+  </si>
+  <si>
+    <t>“explain in step by step these functions”</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,12 +297,45 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -175,7 +358,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -506,11 +689,78 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -557,6 +807,76 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="7" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="15" fontId="7" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -572,26 +892,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,10 +944,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
-          </a:schemeClr>
+          <a:schemeClr val="accent2"/>
         </a:solidFill>
         <a:ln>
           <a:solidFill>
@@ -716,10 +1013,7 @@
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
-          </a:schemeClr>
+          <a:schemeClr val="accent2"/>
         </a:solidFill>
         <a:ln>
           <a:solidFill>
@@ -1440,527 +1734,651 @@
   </sheetPr>
   <dimension ref="B1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="18.21875" style="36" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="36" customWidth="1"/>
-    <col min="4" max="4" width="78" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" style="30" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="30" customWidth="1"/>
+    <col min="4" max="4" width="94" style="2" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" s="37" customFormat="1" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="35" t="s">
+    <row r="2" spans="2:4" s="31" customFormat="1" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="38">
-        <v>46048</v>
-      </c>
-      <c r="C3" s="39">
+    <row r="3" spans="2:4" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="53">
+        <v>45683</v>
+      </c>
+      <c r="C3" s="52">
         <v>2</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="53"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="53"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="53"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="44" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42" t="s">
+    <row r="7" spans="2:4" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="53">
+        <v>45684</v>
+      </c>
+      <c r="C7" s="52">
+        <v>1.5</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="53"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="53"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="45" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="53"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="53">
+        <v>45686</v>
+      </c>
+      <c r="C11" s="52">
+        <v>3</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="53"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="53"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="53"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="47" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="53"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="44" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42" t="s">
+    <row r="16" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="53">
+        <v>46053</v>
+      </c>
+      <c r="C16" s="52">
+        <v>4</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="53"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="53"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="53"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="53"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="53"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="53"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="53"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="53"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="53"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="53"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="48" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="53">
+        <v>46054</v>
+      </c>
+      <c r="C27" s="52">
+        <v>1</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="53"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="53"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="53"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="44" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="42"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="42"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="42"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="42"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="42"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="41"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="42"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="42"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B23" s="41"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="42"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B26" s="41"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="42"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" s="41"/>
-      <c r="C27" s="41"/>
-      <c r="D27" s="42"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B28" s="41"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="42"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="42"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="42"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="42"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="42"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="42"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="42"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B35" s="41"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="42"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="42"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="42"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="42"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B39" s="41"/>
-      <c r="C39" s="41"/>
-      <c r="D39" s="42"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="42"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="42"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B42" s="41"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="42"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="42"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="42"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B45" s="41"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="42"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B46" s="41"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="42"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B47" s="41"/>
-      <c r="C47" s="41"/>
-      <c r="D47" s="42"/>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B48" s="41"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="42"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="42"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B50" s="41"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="42"/>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B51" s="41"/>
-      <c r="C51" s="41"/>
-      <c r="D51" s="42"/>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B52" s="41"/>
-      <c r="C52" s="41"/>
-      <c r="D52" s="42"/>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B53" s="41"/>
-      <c r="C53" s="41"/>
-      <c r="D53" s="42"/>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B54" s="41"/>
-      <c r="C54" s="41"/>
-      <c r="D54" s="42"/>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B55" s="41"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="42"/>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B56" s="41"/>
-      <c r="C56" s="41"/>
-      <c r="D56" s="42"/>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B57" s="41"/>
-      <c r="C57" s="41"/>
-      <c r="D57" s="42"/>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B58" s="41"/>
-      <c r="C58" s="41"/>
-      <c r="D58" s="42"/>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B59" s="41"/>
-      <c r="C59" s="41"/>
-      <c r="D59" s="42"/>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B60" s="41"/>
-      <c r="C60" s="41"/>
-      <c r="D60" s="42"/>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B61" s="41"/>
-      <c r="C61" s="41"/>
-      <c r="D61" s="42"/>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B62" s="41"/>
-      <c r="C62" s="41"/>
-      <c r="D62" s="42"/>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B63" s="41"/>
-      <c r="C63" s="41"/>
-      <c r="D63" s="42"/>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B64" s="41"/>
-      <c r="C64" s="41"/>
-      <c r="D64" s="42"/>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B65" s="41"/>
-      <c r="C65" s="41"/>
-      <c r="D65" s="42"/>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B66" s="41"/>
-      <c r="C66" s="41"/>
-      <c r="D66" s="42"/>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B67" s="41"/>
-      <c r="C67" s="41"/>
-      <c r="D67" s="42"/>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B68" s="41"/>
-      <c r="C68" s="41"/>
-      <c r="D68" s="42"/>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B69" s="41"/>
-      <c r="C69" s="41"/>
-      <c r="D69" s="42"/>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B70" s="41"/>
-      <c r="C70" s="41"/>
-      <c r="D70" s="42"/>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B71" s="41"/>
-      <c r="C71" s="41"/>
-      <c r="D71" s="42"/>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B72" s="41"/>
-      <c r="C72" s="41"/>
-      <c r="D72" s="42"/>
+    <row r="31" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="53">
+        <v>46055</v>
+      </c>
+      <c r="C31" s="52">
+        <v>4</v>
+      </c>
+      <c r="D31" s="41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="53"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="53"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="53"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="53"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="53"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="50" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="53">
+        <v>46056</v>
+      </c>
+      <c r="C37" s="52">
+        <v>3</v>
+      </c>
+      <c r="D37" s="37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="53"/>
+      <c r="C38" s="52"/>
+      <c r="D38" s="37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="53"/>
+      <c r="C39" s="52"/>
+      <c r="D39" s="37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="53"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="53"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="53">
+        <v>46057</v>
+      </c>
+      <c r="C42" s="52">
+        <v>1</v>
+      </c>
+      <c r="D42" s="40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="53"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B44" s="54"/>
+      <c r="C44" s="55"/>
+      <c r="D44" s="51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="33"/>
+    </row>
+    <row r="46" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="33"/>
+    </row>
+    <row r="47" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="33"/>
+    </row>
+    <row r="48" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="33"/>
+    </row>
+    <row r="49" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="33"/>
+    </row>
+    <row r="50" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="33"/>
+    </row>
+    <row r="51" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B51" s="36"/>
+      <c r="C51" s="36"/>
+      <c r="D51" s="33"/>
+    </row>
+    <row r="52" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B52" s="36"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="33"/>
+    </row>
+    <row r="53" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B53" s="36"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="33"/>
+    </row>
+    <row r="54" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B54" s="36"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="33"/>
+    </row>
+    <row r="55" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="33"/>
+    </row>
+    <row r="56" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B56" s="36"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="33"/>
+    </row>
+    <row r="57" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="33"/>
+    </row>
+    <row r="58" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
+      <c r="D58" s="33"/>
+    </row>
+    <row r="59" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="33"/>
+    </row>
+    <row r="60" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="33"/>
+    </row>
+    <row r="61" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B61" s="36"/>
+      <c r="C61" s="36"/>
+      <c r="D61" s="33"/>
+    </row>
+    <row r="62" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B62" s="36"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="33"/>
+    </row>
+    <row r="63" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B63" s="36"/>
+      <c r="C63" s="36"/>
+      <c r="D63" s="33"/>
+    </row>
+    <row r="64" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
+      <c r="D64" s="33"/>
+    </row>
+    <row r="65" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="33"/>
+    </row>
+    <row r="66" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B66" s="36"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="33"/>
+    </row>
+    <row r="67" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B67" s="36"/>
+      <c r="C67" s="36"/>
+      <c r="D67" s="33"/>
+    </row>
+    <row r="68" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B68" s="36"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="33"/>
+    </row>
+    <row r="69" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B69" s="36"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="33"/>
+    </row>
+    <row r="70" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B70" s="36"/>
+      <c r="C70" s="36"/>
+      <c r="D70" s="33"/>
+    </row>
+    <row r="71" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B71" s="36"/>
+      <c r="C71" s="36"/>
+      <c r="D71" s="33"/>
+    </row>
+    <row r="72" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B72" s="36"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="33"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B73" s="41"/>
-      <c r="C73" s="41"/>
-      <c r="D73" s="42"/>
+      <c r="B73" s="32"/>
+      <c r="C73" s="32"/>
+      <c r="D73" s="33"/>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B74" s="41"/>
-      <c r="C74" s="41"/>
-      <c r="D74" s="42"/>
+      <c r="B74" s="32"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="33"/>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B75" s="41"/>
-      <c r="C75" s="41"/>
-      <c r="D75" s="42"/>
+      <c r="B75" s="32"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="33"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B76" s="41"/>
-      <c r="C76" s="41"/>
-      <c r="D76" s="42"/>
+      <c r="B76" s="32"/>
+      <c r="C76" s="32"/>
+      <c r="D76" s="33"/>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B77" s="41"/>
-      <c r="C77" s="41"/>
-      <c r="D77" s="42"/>
+      <c r="B77" s="32"/>
+      <c r="C77" s="32"/>
+      <c r="D77" s="33"/>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B78" s="41"/>
-      <c r="C78" s="41"/>
-      <c r="D78" s="42"/>
+      <c r="B78" s="32"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="33"/>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B79" s="41"/>
-      <c r="C79" s="41"/>
-      <c r="D79" s="42"/>
+      <c r="B79" s="32"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="33"/>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B80" s="41"/>
-      <c r="C80" s="41"/>
-      <c r="D80" s="42"/>
+      <c r="B80" s="32"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="33"/>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B81" s="41"/>
-      <c r="C81" s="41"/>
-      <c r="D81" s="42"/>
+      <c r="B81" s="32"/>
+      <c r="C81" s="32"/>
+      <c r="D81" s="33"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B82" s="41"/>
-      <c r="C82" s="41"/>
-      <c r="D82" s="42"/>
+      <c r="B82" s="32"/>
+      <c r="C82" s="32"/>
+      <c r="D82" s="33"/>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B83" s="41"/>
-      <c r="C83" s="41"/>
-      <c r="D83" s="42"/>
+      <c r="B83" s="32"/>
+      <c r="C83" s="32"/>
+      <c r="D83" s="33"/>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B84" s="41"/>
-      <c r="C84" s="41"/>
-      <c r="D84" s="42"/>
+      <c r="B84" s="32"/>
+      <c r="C84" s="32"/>
+      <c r="D84" s="33"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B85" s="41"/>
-      <c r="C85" s="41"/>
-      <c r="D85" s="42"/>
+      <c r="B85" s="32"/>
+      <c r="C85" s="32"/>
+      <c r="D85" s="33"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B86" s="41"/>
-      <c r="C86" s="41"/>
-      <c r="D86" s="42"/>
+      <c r="B86" s="32"/>
+      <c r="C86" s="32"/>
+      <c r="D86" s="33"/>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B87" s="41"/>
-      <c r="C87" s="41"/>
-      <c r="D87" s="42"/>
+      <c r="B87" s="32"/>
+      <c r="C87" s="32"/>
+      <c r="D87" s="33"/>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B88" s="41"/>
-      <c r="C88" s="41"/>
-      <c r="D88" s="42"/>
+      <c r="B88" s="32"/>
+      <c r="C88" s="32"/>
+      <c r="D88" s="33"/>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B89" s="41"/>
-      <c r="C89" s="41"/>
-      <c r="D89" s="42"/>
+      <c r="B89" s="32"/>
+      <c r="C89" s="32"/>
+      <c r="D89" s="33"/>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B90" s="41"/>
-      <c r="C90" s="41"/>
-      <c r="D90" s="42"/>
+      <c r="B90" s="32"/>
+      <c r="C90" s="32"/>
+      <c r="D90" s="33"/>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B91" s="41"/>
-      <c r="C91" s="41"/>
-      <c r="D91" s="42"/>
+      <c r="B91" s="32"/>
+      <c r="C91" s="32"/>
+      <c r="D91" s="33"/>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B92" s="41"/>
-      <c r="C92" s="41"/>
-      <c r="D92" s="42"/>
+      <c r="B92" s="32"/>
+      <c r="C92" s="32"/>
+      <c r="D92" s="33"/>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B93" s="41"/>
-      <c r="C93" s="41"/>
-      <c r="D93" s="42"/>
+      <c r="B93" s="32"/>
+      <c r="C93" s="32"/>
+      <c r="D93" s="33"/>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B94" s="41"/>
-      <c r="C94" s="41"/>
-      <c r="D94" s="42"/>
+      <c r="B94" s="32"/>
+      <c r="C94" s="32"/>
+      <c r="D94" s="33"/>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B95" s="41"/>
-      <c r="C95" s="41"/>
-      <c r="D95" s="42"/>
+      <c r="B95" s="32"/>
+      <c r="C95" s="32"/>
+      <c r="D95" s="33"/>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B96" s="41"/>
-      <c r="C96" s="41"/>
-      <c r="D96" s="42"/>
+      <c r="B96" s="32"/>
+      <c r="C96" s="32"/>
+      <c r="D96" s="33"/>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B97" s="41"/>
-      <c r="C97" s="41"/>
-      <c r="D97" s="42"/>
+      <c r="B97" s="32"/>
+      <c r="C97" s="32"/>
+      <c r="D97" s="33"/>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B98" s="41"/>
-      <c r="C98" s="41"/>
-      <c r="D98" s="42"/>
+      <c r="B98" s="32"/>
+      <c r="C98" s="32"/>
+      <c r="D98" s="33"/>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B99" s="41"/>
-      <c r="C99" s="41"/>
-      <c r="D99" s="42"/>
+      <c r="B99" s="32"/>
+      <c r="C99" s="32"/>
+      <c r="D99" s="33"/>
     </row>
   </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="C16:C26"/>
+    <mergeCell ref="B16:B26"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="C37:C41"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C42:C44"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1973,7 +2391,7 @@
   <dimension ref="D2:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1989,36 +2407,36 @@
   <sheetData>
     <row r="2" spans="4:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="59" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="30" t="s">
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="30" t="s">
+      <c r="K3" s="57"/>
+      <c r="L3" s="57"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="32"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="58"/>
       <c r="R3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="4:18" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D4" s="34"/>
+      <c r="D4" s="60"/>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
update the progress report and worklog
</commit_message>
<xml_diff>
--- a/DocumentsAndReports/0. WorkLog_Charts.xlsx
+++ b/DocumentsAndReports/0. WorkLog_Charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qhung\Videos\CSIS4495 - Applied Research  Project\W26_4495_S2_HughT\DocumentsAndReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408518D8-E9CA-43B5-B9FA-37D5CA288550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC09D5F-14B7-4D81-A819-14EBD36FFF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="972" yWindow="696" windowWidth="21600" windowHeight="11232" xr2:uid="{E067A1E6-0DC4-42DD-AAF8-D95EFF7A112F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E067A1E6-0DC4-42DD-AAF8-D95EFF7A112F}"/>
   </bookViews>
   <sheets>
     <sheet name="Work_Log" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
     <t>January</t>
   </si>
@@ -253,6 +253,30 @@
   </si>
   <si>
     <t>“explain in step by step these functions”</t>
+  </si>
+  <si>
+    <t>- Updated the progress report</t>
+  </si>
+  <si>
+    <t>- Research about FastAPI to connect html front-end with backend by python</t>
+  </si>
+  <si>
+    <t>“how can use fastapi to connect a html frontend and backend in python”</t>
+  </si>
+  <si>
+    <t>“explain these api in details, line by line”</t>
+  </si>
+  <si>
+    <t>- Researched front-end's frameworks for uploading the dataset</t>
+  </si>
+  <si>
+    <t>“which framework works best with html + fastApi?”</t>
+  </si>
+  <si>
+    <t>“compare bootstrap and tailwind”</t>
+  </si>
+  <si>
+    <t>“why should use jinja template?, what if not using it”</t>
   </si>
 </sst>
 </file>
@@ -760,7 +784,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -864,33 +888,47 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="15" fontId="7" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="15" fontId="7" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1734,8 +1772,8 @@
   </sheetPr>
   <dimension ref="B1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1760,10 +1798,10 @@
       </c>
     </row>
     <row r="3" spans="2:4" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="53">
+      <c r="B3" s="54">
         <v>45683</v>
       </c>
-      <c r="C3" s="52">
+      <c r="C3" s="53">
         <v>2</v>
       </c>
       <c r="D3" s="37" t="s">
@@ -1771,31 +1809,31 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="53"/>
-      <c r="C4" s="52"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="53"/>
       <c r="D4" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="53"/>
-      <c r="C5" s="52"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="53"/>
       <c r="D5" s="43" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="53"/>
-      <c r="C6" s="52"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="53"/>
       <c r="D6" s="44" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="53">
+      <c r="B7" s="54">
         <v>45684</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="53">
         <v>1.5</v>
       </c>
       <c r="D7" s="38" t="s">
@@ -1803,31 +1841,31 @@
       </c>
     </row>
     <row r="8" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="53"/>
-      <c r="C8" s="52"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="39" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="53"/>
-      <c r="C9" s="52"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="53"/>
       <c r="D9" s="45" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="53"/>
-      <c r="C10" s="52"/>
+      <c r="B10" s="54"/>
+      <c r="C10" s="53"/>
       <c r="D10" s="46" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="53">
+      <c r="B11" s="54">
         <v>45686</v>
       </c>
-      <c r="C11" s="52">
+      <c r="C11" s="53">
         <v>3</v>
       </c>
       <c r="D11" s="37" t="s">
@@ -1835,38 +1873,38 @@
       </c>
     </row>
     <row r="12" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="53"/>
-      <c r="C12" s="52"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="53"/>
       <c r="D12" s="37" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="53"/>
-      <c r="C13" s="52"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="53"/>
       <c r="D13" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="53"/>
-      <c r="C14" s="52"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="53"/>
       <c r="D14" s="47" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="53"/>
-      <c r="C15" s="52"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="53"/>
       <c r="D15" s="44" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="53">
+      <c r="B16" s="54">
         <v>46053</v>
       </c>
-      <c r="C16" s="52">
+      <c r="C16" s="53">
         <v>4</v>
       </c>
       <c r="D16" s="40" t="s">
@@ -1874,80 +1912,80 @@
       </c>
     </row>
     <row r="17" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="53"/>
-      <c r="C17" s="52"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="53"/>
       <c r="D17" s="37" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="53"/>
-      <c r="C18" s="52"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="53"/>
       <c r="D18" s="37" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="53"/>
-      <c r="C19" s="52"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="53"/>
       <c r="D19" s="37" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="53"/>
-      <c r="C20" s="52"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="53"/>
       <c r="D20" s="37" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="53"/>
-      <c r="C21" s="52"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="53"/>
       <c r="D21" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="53"/>
-      <c r="C22" s="52"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="53"/>
       <c r="D22" s="47" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="53"/>
-      <c r="C23" s="52"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="43" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="53"/>
-      <c r="C24" s="52"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="53"/>
       <c r="D24" s="43" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="53"/>
-      <c r="C25" s="52"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="53"/>
       <c r="D25" s="43" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="53"/>
-      <c r="C26" s="52"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="53"/>
       <c r="D26" s="48" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="53">
+      <c r="B27" s="54">
         <v>46054</v>
       </c>
-      <c r="C27" s="52">
+      <c r="C27" s="53">
         <v>1</v>
       </c>
       <c r="D27" s="37" t="s">
@@ -1955,31 +1993,31 @@
       </c>
     </row>
     <row r="28" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="53"/>
-      <c r="C28" s="52"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="53"/>
       <c r="D28" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="53"/>
-      <c r="C29" s="52"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="53"/>
       <c r="D29" s="43" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="53"/>
-      <c r="C30" s="52"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="53"/>
       <c r="D30" s="44" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="53">
+      <c r="B31" s="54">
         <v>46055</v>
       </c>
-      <c r="C31" s="52">
+      <c r="C31" s="53">
         <v>4</v>
       </c>
       <c r="D31" s="41" t="s">
@@ -1987,45 +2025,45 @@
       </c>
     </row>
     <row r="32" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="53"/>
-      <c r="C32" s="52"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="53"/>
       <c r="D32" s="42" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="53"/>
-      <c r="C33" s="52"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="53"/>
       <c r="D33" s="42" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="53"/>
-      <c r="C34" s="52"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="53"/>
       <c r="D34" s="42" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="53"/>
-      <c r="C35" s="52"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="53"/>
       <c r="D35" s="49" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="53"/>
-      <c r="C36" s="52"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="53"/>
       <c r="D36" s="50" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="53">
+      <c r="B37" s="54">
         <v>46056</v>
       </c>
-      <c r="C37" s="52">
+      <c r="C37" s="53">
         <v>3</v>
       </c>
       <c r="D37" s="37" t="s">
@@ -2033,107 +2071,135 @@
       </c>
     </row>
     <row r="38" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="53"/>
-      <c r="C38" s="52"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="53"/>
       <c r="D38" s="37" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="53"/>
-      <c r="C39" s="52"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="53"/>
       <c r="D39" s="37" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="53"/>
-      <c r="C40" s="52"/>
+      <c r="B40" s="54"/>
+      <c r="C40" s="53"/>
       <c r="D40" s="43" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="53"/>
-      <c r="C41" s="52"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="53"/>
       <c r="D41" s="44" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="53">
+      <c r="B42" s="54">
         <v>46057</v>
       </c>
-      <c r="C42" s="52">
-        <v>1</v>
+      <c r="C42" s="53">
+        <v>4</v>
       </c>
       <c r="D42" s="40" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="53"/>
-      <c r="C43" s="52"/>
+      <c r="B43" s="54"/>
+      <c r="C43" s="53"/>
       <c r="D43" s="37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B44" s="54"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="51" t="s">
+      <c r="C44" s="53"/>
+      <c r="D44" s="44" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B45" s="35"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="33"/>
+      <c r="B45" s="62">
+        <v>46059</v>
+      </c>
+      <c r="C45" s="63">
+        <v>2</v>
+      </c>
+      <c r="D45" s="52" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="46" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B46" s="35"/>
       <c r="C46" s="35"/>
-      <c r="D46" s="33"/>
+      <c r="D46" s="51" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="47" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B47" s="35"/>
       <c r="C47" s="35"/>
-      <c r="D47" s="33"/>
+      <c r="D47" s="37" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="48" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B48" s="35"/>
       <c r="C48" s="35"/>
-      <c r="D48" s="33"/>
-    </row>
-    <row r="49" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="33"/>
+      <c r="D48" s="44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="64"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="48" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="50" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="33"/>
+      <c r="B50" s="62">
+        <v>46061</v>
+      </c>
+      <c r="C50" s="60">
+        <v>1.5</v>
+      </c>
+      <c r="D50" s="61" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="51" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B51" s="36"/>
       <c r="C51" s="36"/>
-      <c r="D51" s="33"/>
+      <c r="D51" s="37" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="52" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B52" s="36"/>
       <c r="C52" s="36"/>
-      <c r="D52" s="33"/>
+      <c r="D52" s="44" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="53" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B53" s="36"/>
       <c r="C53" s="36"/>
-      <c r="D53" s="33"/>
+      <c r="D53" s="44" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="54" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B54" s="36"/>
       <c r="C54" s="36"/>
-      <c r="D54" s="33"/>
+      <c r="D54" s="44" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="55" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B55" s="36"/>
@@ -2390,7 +2456,7 @@
   </sheetPr>
   <dimension ref="D2:R11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2407,36 +2473,36 @@
   <sheetData>
     <row r="2" spans="4:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="4:18" x14ac:dyDescent="0.3">
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="58" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="56" t="s">
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="56" t="s">
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="57"/>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="58"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="57"/>
       <c r="R3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="4:18" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D4" s="60"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
submit the progress report 1
</commit_message>
<xml_diff>
--- a/DocumentsAndReports/0. WorkLog_Charts.xlsx
+++ b/DocumentsAndReports/0. WorkLog_Charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qhung\Videos\CSIS4495 - Applied Research  Project\W26_4495_S2_HughT\DocumentsAndReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC09D5F-14B7-4D81-A819-14EBD36FFF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9A8528-F9A3-49F1-A1D2-2BFC803C95B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E067A1E6-0DC4-42DD-AAF8-D95EFF7A112F}"/>
   </bookViews>
@@ -784,7 +784,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -845,9 +845,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -894,6 +891,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -915,20 +915,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="7" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="7" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="7" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="15" fontId="7" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1772,8 +1776,8 @@
   </sheetPr>
   <dimension ref="B1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1804,28 +1808,28 @@
       <c r="C3" s="53">
         <v>2</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="36" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="54"/>
       <c r="C4" s="53"/>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="36" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="54"/>
       <c r="C5" s="53"/>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="42" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="54"/>
       <c r="C6" s="53"/>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="43" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1836,28 +1840,28 @@
       <c r="C7" s="53">
         <v>1.5</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="37" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="54"/>
       <c r="C8" s="53"/>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="38" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="54"/>
       <c r="C9" s="53"/>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="44" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="54"/>
       <c r="C10" s="53"/>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="45" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1868,35 +1872,35 @@
       <c r="C11" s="53">
         <v>3</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="36" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="54"/>
       <c r="C12" s="53"/>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="36" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="54"/>
       <c r="C13" s="53"/>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="36" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="54"/>
       <c r="C14" s="53"/>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="46" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="54"/>
       <c r="C15" s="53"/>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="43" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1907,77 +1911,77 @@
       <c r="C16" s="53">
         <v>4</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="39" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="54"/>
       <c r="C17" s="53"/>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="36" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="54"/>
       <c r="C18" s="53"/>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="36" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="54"/>
       <c r="C19" s="53"/>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="36" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="54"/>
       <c r="C20" s="53"/>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="36" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="54"/>
       <c r="C21" s="53"/>
-      <c r="D21" s="37" t="s">
+      <c r="D21" s="36" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="54"/>
       <c r="C22" s="53"/>
-      <c r="D22" s="47" t="s">
+      <c r="D22" s="46" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="54"/>
       <c r="C23" s="53"/>
-      <c r="D23" s="43" t="s">
+      <c r="D23" s="42" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="54"/>
       <c r="C24" s="53"/>
-      <c r="D24" s="43" t="s">
+      <c r="D24" s="42" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="54"/>
       <c r="C25" s="53"/>
-      <c r="D25" s="43" t="s">
+      <c r="D25" s="42" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="54"/>
       <c r="C26" s="53"/>
-      <c r="D26" s="48" t="s">
+      <c r="D26" s="47" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1988,28 +1992,28 @@
       <c r="C27" s="53">
         <v>1</v>
       </c>
-      <c r="D27" s="37" t="s">
+      <c r="D27" s="36" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="54"/>
       <c r="C28" s="53"/>
-      <c r="D28" s="37" t="s">
+      <c r="D28" s="36" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="54"/>
       <c r="C29" s="53"/>
-      <c r="D29" s="43" t="s">
+      <c r="D29" s="42" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="54"/>
       <c r="C30" s="53"/>
-      <c r="D30" s="44" t="s">
+      <c r="D30" s="43" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2020,42 +2024,42 @@
       <c r="C31" s="53">
         <v>4</v>
       </c>
-      <c r="D31" s="41" t="s">
+      <c r="D31" s="40" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="54"/>
       <c r="C32" s="53"/>
-      <c r="D32" s="42" t="s">
+      <c r="D32" s="41" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="54"/>
       <c r="C33" s="53"/>
-      <c r="D33" s="42" t="s">
+      <c r="D33" s="41" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="54"/>
       <c r="C34" s="53"/>
-      <c r="D34" s="42" t="s">
+      <c r="D34" s="41" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="54"/>
       <c r="C35" s="53"/>
-      <c r="D35" s="49" t="s">
+      <c r="D35" s="48" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="54"/>
       <c r="C36" s="53"/>
-      <c r="D36" s="50" t="s">
+      <c r="D36" s="49" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2066,35 +2070,35 @@
       <c r="C37" s="53">
         <v>3</v>
       </c>
-      <c r="D37" s="37" t="s">
+      <c r="D37" s="36" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="54"/>
       <c r="C38" s="53"/>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="36" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="54"/>
       <c r="C39" s="53"/>
-      <c r="D39" s="37" t="s">
+      <c r="D39" s="36" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="54"/>
       <c r="C40" s="53"/>
-      <c r="D40" s="43" t="s">
+      <c r="D40" s="42" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="54"/>
       <c r="C41" s="53"/>
-      <c r="D41" s="44" t="s">
+      <c r="D41" s="43" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2105,190 +2109,190 @@
       <c r="C42" s="53">
         <v>4</v>
       </c>
-      <c r="D42" s="40" t="s">
+      <c r="D42" s="39" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="54"/>
       <c r="C43" s="53"/>
-      <c r="D43" s="37" t="s">
+      <c r="D43" s="36" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B44" s="54"/>
       <c r="C44" s="53"/>
-      <c r="D44" s="44" t="s">
+      <c r="D44" s="43" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B45" s="62">
+      <c r="B45" s="61">
         <v>46059</v>
       </c>
-      <c r="C45" s="63">
+      <c r="C45" s="64">
         <v>2</v>
       </c>
-      <c r="D45" s="52" t="s">
+      <c r="D45" s="51" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B46" s="35"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="51" t="s">
+      <c r="B46" s="62"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="50" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="37" t="s">
+      <c r="B47" s="62"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="36" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B48" s="35"/>
-      <c r="C48" s="35"/>
-      <c r="D48" s="44" t="s">
+      <c r="B48" s="62"/>
+      <c r="C48" s="65"/>
+      <c r="D48" s="43" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="49" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="64"/>
-      <c r="C49" s="64"/>
-      <c r="D49" s="48" t="s">
+      <c r="B49" s="63"/>
+      <c r="C49" s="66"/>
+      <c r="D49" s="47" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B50" s="62">
+      <c r="B50" s="61">
         <v>46061</v>
       </c>
-      <c r="C50" s="60">
+      <c r="C50" s="64">
         <v>1.5</v>
       </c>
-      <c r="D50" s="61" t="s">
+      <c r="D50" s="51" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="37" t="s">
+      <c r="B51" s="62"/>
+      <c r="C51" s="65"/>
+      <c r="D51" s="36" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="52" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="44" t="s">
+      <c r="B52" s="62"/>
+      <c r="C52" s="65"/>
+      <c r="D52" s="43" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="44" t="s">
+      <c r="B53" s="62"/>
+      <c r="C53" s="65"/>
+      <c r="D53" s="43" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="44" t="s">
+    <row r="54" spans="2:4" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="63"/>
+      <c r="C54" s="66"/>
+      <c r="D54" s="47" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="55" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="33"/>
+      <c r="B55" s="52"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="60"/>
     </row>
     <row r="56" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="35"/>
       <c r="D56" s="33"/>
     </row>
     <row r="57" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
+      <c r="B57" s="35"/>
+      <c r="C57" s="35"/>
       <c r="D57" s="33"/>
     </row>
     <row r="58" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="35"/>
       <c r="D58" s="33"/>
     </row>
     <row r="59" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="35"/>
       <c r="D59" s="33"/>
     </row>
     <row r="60" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="35"/>
       <c r="D60" s="33"/>
     </row>
     <row r="61" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="35"/>
       <c r="D61" s="33"/>
     </row>
     <row r="62" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="35"/>
       <c r="D62" s="33"/>
     </row>
     <row r="63" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B63" s="36"/>
-      <c r="C63" s="36"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="35"/>
       <c r="D63" s="33"/>
     </row>
     <row r="64" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B64" s="36"/>
-      <c r="C64" s="36"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="35"/>
       <c r="D64" s="33"/>
     </row>
     <row r="65" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B65" s="36"/>
-      <c r="C65" s="36"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="35"/>
       <c r="D65" s="33"/>
     </row>
     <row r="66" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B66" s="36"/>
-      <c r="C66" s="36"/>
+      <c r="B66" s="35"/>
+      <c r="C66" s="35"/>
       <c r="D66" s="33"/>
     </row>
     <row r="67" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B67" s="36"/>
-      <c r="C67" s="36"/>
+      <c r="B67" s="35"/>
+      <c r="C67" s="35"/>
       <c r="D67" s="33"/>
     </row>
     <row r="68" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
+      <c r="B68" s="35"/>
+      <c r="C68" s="35"/>
       <c r="D68" s="33"/>
     </row>
     <row r="69" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B69" s="36"/>
-      <c r="C69" s="36"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="35"/>
       <c r="D69" s="33"/>
     </row>
     <row r="70" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B70" s="36"/>
-      <c r="C70" s="36"/>
+      <c r="B70" s="35"/>
+      <c r="C70" s="35"/>
       <c r="D70" s="33"/>
     </row>
     <row r="71" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B71" s="36"/>
-      <c r="C71" s="36"/>
+      <c r="B71" s="35"/>
+      <c r="C71" s="35"/>
       <c r="D71" s="33"/>
     </row>
     <row r="72" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B72" s="36"/>
-      <c r="C72" s="36"/>
+      <c r="B72" s="35"/>
+      <c r="C72" s="35"/>
       <c r="D72" s="33"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.3">
@@ -2427,7 +2431,17 @@
       <c r="D99" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="20">
+    <mergeCell ref="B45:B49"/>
+    <mergeCell ref="C45:C49"/>
+    <mergeCell ref="B50:B54"/>
+    <mergeCell ref="C50:C54"/>
+    <mergeCell ref="C31:C36"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="C37:C41"/>
+    <mergeCell ref="B37:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C42:C44"/>
     <mergeCell ref="C16:C26"/>
     <mergeCell ref="B16:B26"/>
     <mergeCell ref="C27:C30"/>
@@ -2438,12 +2452,6 @@
     <mergeCell ref="C7:C10"/>
     <mergeCell ref="B11:B15"/>
     <mergeCell ref="C11:C15"/>
-    <mergeCell ref="C31:C36"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="C37:C41"/>
-    <mergeCell ref="B37:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C42:C44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>